<commit_message>
completed modules of actions attachments
</commit_message>
<xml_diff>
--- a/Excel/TigerKrionDataSheet.xlsx
+++ b/Excel/TigerKrionDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TWINUser13\eclipse-workspace\Automation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C8265-D491-4428-97E8-5F4DDC348463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E6C409-27E6-4CEE-9430-A147F38D3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="4" activeTab="4" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,15 @@
     <sheet name="Add Project" sheetId="5" r:id="rId3"/>
     <sheet name="Assign Role" sheetId="6" r:id="rId4"/>
     <sheet name="Workflow" sheetId="7" r:id="rId5"/>
-    <sheet name="Teams Module" sheetId="3" r:id="rId6"/>
-    <sheet name="Role Module" sheetId="2" r:id="rId7"/>
+    <sheet name="Approval Steps" sheetId="8" r:id="rId6"/>
+    <sheet name="Add Review" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="Add Issue" sheetId="11" r:id="rId9"/>
+    <sheet name="Add RFA" sheetId="12" r:id="rId10"/>
+    <sheet name="Add Meeting" sheetId="13" r:id="rId11"/>
+    <sheet name="Add BOMBOQ" sheetId="14" r:id="rId12"/>
+    <sheet name="Teams Module" sheetId="3" r:id="rId13"/>
+    <sheet name="Role Module" sheetId="2" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="231">
   <si>
     <t>Login Email</t>
   </si>
@@ -174,9 +181,6 @@
     <t>SelectTheCategory</t>
   </si>
   <si>
-    <t>RFA</t>
-  </si>
-  <si>
     <t>Role For Group</t>
   </si>
   <si>
@@ -234,17 +238,506 @@
     <t>nsdkfhalkdfhlakjf</t>
   </si>
   <si>
-    <t>In-Active</t>
-  </si>
-  <si>
     <t>Approved</t>
+  </si>
+  <si>
+    <t>Test Project</t>
+  </si>
+  <si>
+    <t>Approval Type</t>
+  </si>
+  <si>
+    <t>Step Name</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>One Step Approval</t>
+  </si>
+  <si>
+    <t>Four Step Approval</t>
+  </si>
+  <si>
+    <t>Five Step Approval</t>
+  </si>
+  <si>
+    <t>Six Step Approval</t>
+  </si>
+  <si>
+    <t>Seven Step Approval</t>
+  </si>
+  <si>
+    <t>Manik</t>
+  </si>
+  <si>
+    <t>gopi</t>
+  </si>
+  <si>
+    <t>sudhkar</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>awer</t>
+  </si>
+  <si>
+    <t>wer</t>
+  </si>
+  <si>
+    <t>asdfasjdflkjasdf</t>
+  </si>
+  <si>
+    <t>aoewrutoipjwer</t>
+  </si>
+  <si>
+    <t>asdnfhoiqwheriu</t>
+  </si>
+  <si>
+    <t>ahkGSdfkhablekjf</t>
+  </si>
+  <si>
+    <t>asdhfwi</t>
+  </si>
+  <si>
+    <t>saw</t>
+  </si>
+  <si>
+    <t>asfg</t>
+  </si>
+  <si>
+    <t>dsfhg</t>
+  </si>
+  <si>
+    <t>sdg</t>
+  </si>
+  <si>
+    <t>xgv</t>
+  </si>
+  <si>
+    <t>satg3w4</t>
+  </si>
+  <si>
+    <t>asdfw</t>
+  </si>
+  <si>
+    <t>asgft</t>
+  </si>
+  <si>
+    <t>asgw</t>
+  </si>
+  <si>
+    <t>werwsaetr</t>
+  </si>
+  <si>
+    <t>asdfwe</t>
+  </si>
+  <si>
+    <t>asdgfasf</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>asdfwer</t>
+  </si>
+  <si>
+    <t>sdfasfw</t>
+  </si>
+  <si>
+    <t>asdfgwer</t>
+  </si>
+  <si>
+    <t>User Group</t>
+  </si>
+  <si>
+    <t>kker</t>
+  </si>
+  <si>
+    <t>this is good</t>
+  </si>
+  <si>
+    <t>ok ok</t>
+  </si>
+  <si>
+    <t>ujkoj</t>
+  </si>
+  <si>
+    <t>Approver Two</t>
+  </si>
+  <si>
+    <t>Parent Review</t>
+  </si>
+  <si>
+    <t>Review Code</t>
+  </si>
+  <si>
+    <t>Review Name</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Start Month</t>
+  </si>
+  <si>
+    <t>Start Year</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>End Month</t>
+  </si>
+  <si>
+    <t>End Year</t>
+  </si>
+  <si>
+    <t>Workflow</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Estimate Cost</t>
+  </si>
+  <si>
+    <t>Actual Cost</t>
+  </si>
+  <si>
+    <t>asdbfjasdfkjbaskjdfakjsdf</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Attachfile</t>
+  </si>
+  <si>
+    <t>0001-XXXX-XX01-RVW-0001-A-P01.11</t>
+  </si>
+  <si>
+    <t>RFIs</t>
+  </si>
+  <si>
+    <t>0001-XXXX-XX01-RFI-0001-A-P01.81</t>
+  </si>
+  <si>
+    <t>0001-XXXX-XX01-RVW-0001-A-P01.21 - Gopal</t>
+  </si>
+  <si>
+    <t>Goki</t>
+  </si>
+  <si>
+    <t>Issue Code</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Due Month</t>
+  </si>
+  <si>
+    <t>Due Year</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>0001-XXXX-XX01-ISS-0001-A-P01.51</t>
+  </si>
+  <si>
+    <t>Modiji</t>
+  </si>
+  <si>
+    <t>sadfasdfasdf</t>
+  </si>
+  <si>
+    <t>Placement</t>
+  </si>
+  <si>
+    <t>Root Cause</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Bed room</t>
+  </si>
+  <si>
+    <t>Patrik</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Painter</t>
+  </si>
+  <si>
+    <t>Upload Images</t>
+  </si>
+  <si>
+    <t>C:\Users\TWINUser13\Pictures\err3.png</t>
+  </si>
+  <si>
+    <t>0001-XXXX-XX01-ISS-0001-A-P01.31</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>0001-XXXX-XX01-RFA-0001-A-P01.31</t>
+  </si>
+  <si>
+    <t>RFA Code</t>
+  </si>
+  <si>
+    <t>RFA Name</t>
+  </si>
+  <si>
+    <t>Magesh</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>RFA Yuva</t>
+  </si>
+  <si>
+    <t>Meeting Start Date</t>
+  </si>
+  <si>
+    <t>Meeting Start Month</t>
+  </si>
+  <si>
+    <t>Meeting Start Year</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>AM/PM</t>
+  </si>
+  <si>
+    <t>Duration Hours</t>
+  </si>
+  <si>
+    <t>Duration Minutes</t>
+  </si>
+  <si>
+    <t>Project Discussion</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>asdfjgbasdkjfbaksjdf</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Enter Notes</t>
+  </si>
+  <si>
+    <t>Every one should attend the meeting its very very important</t>
+  </si>
+  <si>
+    <t>I need this persons to work</t>
+  </si>
+  <si>
+    <t>which is mentioned below</t>
+  </si>
+  <si>
+    <t>raja</t>
+  </si>
+  <si>
+    <t>roja</t>
+  </si>
+  <si>
+    <t>tata</t>
+  </si>
+  <si>
+    <t>brilla</t>
+  </si>
+  <si>
+    <t>gates</t>
+  </si>
+  <si>
+    <t>tim cook</t>
+  </si>
+  <si>
+    <t>steve</t>
+  </si>
+  <si>
+    <t>Select users</t>
+  </si>
+  <si>
+    <t>Select user groups</t>
+  </si>
+  <si>
+    <t>User Kamal</t>
+  </si>
+  <si>
+    <t>Vignesh S</t>
+  </si>
+  <si>
+    <t>Appover One</t>
+  </si>
+  <si>
+    <t>Parent BOM</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Estimated Quantity</t>
+  </si>
+  <si>
+    <t>Estimated Price Per Unit</t>
+  </si>
+  <si>
+    <t>Estimated Total</t>
+  </si>
+  <si>
+    <t>Ordered Quantity</t>
+  </si>
+  <si>
+    <t>Quoted Price Per Unit</t>
+  </si>
+  <si>
+    <t>Quoted Total</t>
+  </si>
+  <si>
+    <t>Actual Quantity</t>
+  </si>
+  <si>
+    <t>Actual Price Per Unit</t>
+  </si>
+  <si>
+    <t>Actual Total</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>GUID</t>
+  </si>
+  <si>
+    <t>QR Code</t>
+  </si>
+  <si>
+    <t>Property Name</t>
+  </si>
+  <si>
+    <t>Property Value</t>
+  </si>
+  <si>
+    <t>0001-XXXX-XX01-BOM-0001-A-P01.51</t>
+  </si>
+  <si>
+    <t>Deepak</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>sq.m</t>
+  </si>
+  <si>
+    <t>asdfasdfasdfewrewfasdf</t>
+  </si>
+  <si>
+    <t>sadfasdf234234sdf</t>
+  </si>
+  <si>
+    <t>KKM soft</t>
+  </si>
+  <si>
+    <t>Vasu</t>
+  </si>
+  <si>
+    <t>C:\Users\TWINUser13\Downloads\QR.png</t>
+  </si>
+  <si>
+    <t>krion</t>
+  </si>
+  <si>
+    <t>auto cad</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>moniter</t>
+  </si>
+  <si>
+    <t>cpu</t>
+  </si>
+  <si>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>consulting</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>5400 laptop</t>
+  </si>
+  <si>
+    <t>dell123</t>
+  </si>
+  <si>
+    <t>clolur</t>
+  </si>
+  <si>
+    <t>64bit process</t>
+  </si>
+  <si>
+    <t>kyes</t>
+  </si>
+  <si>
+    <t>Select parent BOM/BOQ</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Select the parent review</t>
+  </si>
+  <si>
+    <t>Approver Three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +761,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -289,7 +787,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -312,16 +810,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -797,6 +1324,593 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D12559-3BEC-4A49-9DD8-38E929692E89}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="46.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>2007</v>
+      </c>
+      <c r="J2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A118D3E-EF0D-4CA3-9124-14D28D6EC87B}">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="36.140625" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="38.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="16" max="16" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>173</v>
+      </c>
+      <c r="L4" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D35D846-25C7-41D6-9730-C7B818D35A81}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+    <col min="18" max="18" width="35.7109375" customWidth="1"/>
+    <col min="19" max="19" width="25.85546875" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>2.0144445484800002</v>
+      </c>
+      <c r="I2">
+        <v>550</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>2.3666</v>
+      </c>
+      <c r="M2">
+        <v>59</v>
+      </c>
+      <c r="N2">
+        <v>5.4164869580000001</v>
+      </c>
+      <c r="P2" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>208</v>
+      </c>
+      <c r="R2" t="s">
+        <v>211</v>
+      </c>
+      <c r="S2" t="s">
+        <v>209</v>
+      </c>
+      <c r="T2">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>212</v>
+      </c>
+      <c r="T3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>213</v>
+      </c>
+      <c r="T4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>215</v>
+      </c>
+      <c r="T6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>216</v>
+      </c>
+      <c r="T7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>217</v>
+      </c>
+      <c r="T8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>218</v>
+      </c>
+      <c r="T9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C028904-DB84-44AB-AC47-D5B3C226FCB9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D18E19-C11D-415E-BF4F-6B77669DD300}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2316852B-BD5D-4CCB-B9B7-E47F42C84E7D}">
   <dimension ref="A1:G2"/>
@@ -839,10 +1953,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081DB40F-4E4E-4B24-8430-969987B28590}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +2085,15 @@
         <v>41</v>
       </c>
     </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" display="https://tiger.krion6d.com/projects/design/list/344/dashboard" xr:uid="{933BB396-1829-4A52-A1B9-DF13831E0E19}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -981,7 +2103,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,10 +2122,10 @@
         <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -1028,37 +2150,40 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1068,10 +2193,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A2A67-EB9E-4636-A126-D12A8CADACD9}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,52 +2208,120 @@
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>68</v>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" t="s">
+        <v>230</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1137,31 +2330,88 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C028904-DB84-44AB-AC47-D5B3C226FCB9}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5625B-566F-4BA1-B003-A9962CF5B7B3}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1170,40 +2420,606 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D18E19-C11D-415E-BF4F-6B77669DD300}">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D129D65-5A95-4867-A578-DEF4C36C49F1}">
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>229</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>1999</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>2024</v>
+      </c>
+      <c r="K2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2">
+        <v>1200</v>
+      </c>
+      <c r="N2">
+        <v>2400</v>
+      </c>
+      <c r="O2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BA4434-B7C4-4B27-93F0-54C91FF35C7F}">
+  <dimension ref="B6:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A9AD65-B56F-4227-A9C8-DB5B0B54CBC4}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="41.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>2024</v>
+      </c>
+      <c r="J2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" t="s">
+        <v>145</v>
+      </c>
+      <c r="M2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" t="s">
+        <v>144</v>
+      </c>
+      <c r="O2">
+        <v>1234</v>
+      </c>
+      <c r="P2">
+        <v>2100</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>147</v>
+      </c>
+      <c r="R2" t="s">
+        <v>149</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>